<commit_message>
multiple tries for companyname clicking
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -157,7 +157,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -526,7 +526,7 @@
     <col min="8" max="8" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>